<commit_message>
Updated comparision of agglomeration
</commit_message>
<xml_diff>
--- a/Results_and_scripts_ps/agglomeration_comparision.xlsx
+++ b/Results_and_scripts_ps/agglomeration_comparision.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
   <si>
     <t>constants</t>
   </si>
@@ -183,7 +183,10 @@
     <t>case 11</t>
   </si>
   <si>
-    <t>Vastaava log-normaali jakauma lopussa: gsd=1,6691, µ=9e-9, N=Ntot(end)</t>
+    <t>Tämä jakauma on hieman erilainen kuin todellinen jakauma lopussa.</t>
+  </si>
+  <si>
+    <t>Vastaava log-normaali jakauma lopussa: gsd=1,6691, µ=9e-9, N=Ntot(end).</t>
   </si>
 </sst>
 </file>
@@ -627,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="V29" sqref="V29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1750,7 +1753,7 @@
         <v>54</v>
       </c>
       <c r="S25" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="T25" s="10"/>
     </row>
@@ -1785,6 +1788,9 @@
       <c r="P26" s="5">
         <f t="shared" si="1"/>
         <v>2.2127790640149243E-8</v>
+      </c>
+      <c r="S26" s="10" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="5:26" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
New agglomeration tests and documentation
</commit_message>
<xml_diff>
--- a/Results_and_scripts_ps/agglomeration_comparision.xlsx
+++ b/Results_and_scripts_ps/agglomeration_comparision.xlsx
@@ -639,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1982,15 +1982,15 @@
         <v>1</v>
       </c>
       <c r="M35" s="10">
-        <f>V3/U3</f>
+        <f t="shared" ref="M35:M45" si="6">V3/U3</f>
         <v>4.0681357968422374</v>
       </c>
       <c r="N35" s="10">
-        <f>P20/U3</f>
+        <f t="shared" ref="N35:N45" si="7">P20/U3</f>
         <v>3.8659559847566682</v>
       </c>
       <c r="O35" s="10">
-        <f t="shared" ref="O35:O45" si="6">ABS(N35-M35)/N35*100</f>
+        <f t="shared" ref="O35:O45" si="8">ABS(N35-M35)/N35*100</f>
         <v>5.2297494560920299</v>
       </c>
     </row>
@@ -2015,15 +2015,15 @@
         <v>2</v>
       </c>
       <c r="M36" s="10">
-        <f>V4/U4</f>
+        <f t="shared" si="6"/>
         <v>3.8114270757137709</v>
       </c>
       <c r="N36" s="10">
-        <f>P21/U4</f>
+        <f t="shared" si="7"/>
         <v>3.6309061561084972</v>
       </c>
       <c r="O36" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>4.9717869821992577</v>
       </c>
     </row>
@@ -2048,15 +2048,15 @@
         <v>3</v>
       </c>
       <c r="M37" s="10">
-        <f>V5/U5</f>
+        <f t="shared" si="6"/>
         <v>3.7907764093482501</v>
       </c>
       <c r="N37" s="10">
-        <f>P22/U5</f>
+        <f t="shared" si="7"/>
         <v>3.6309061561084972</v>
       </c>
       <c r="O37" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>4.4030400777721379</v>
       </c>
     </row>
@@ -2081,15 +2081,15 @@
         <v>4</v>
       </c>
       <c r="M38" s="10">
-        <f>V6/U6</f>
+        <f t="shared" si="6"/>
         <v>3.7691382988321687</v>
       </c>
       <c r="N38" s="10">
-        <f>P23/U6</f>
+        <f t="shared" si="7"/>
         <v>3.6165699669764839</v>
       </c>
       <c r="O38" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>4.2185920153297776</v>
       </c>
     </row>
@@ -2114,15 +2114,15 @@
         <v>5</v>
       </c>
       <c r="M39" s="10">
-        <f>V7/U7</f>
+        <f t="shared" si="6"/>
         <v>8.6013955211821376</v>
       </c>
       <c r="N39" s="10">
-        <f>P24/U7</f>
+        <f t="shared" si="7"/>
         <v>8.3283923556629311</v>
       </c>
       <c r="O39" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3.2779815582724874</v>
       </c>
     </row>
@@ -2147,15 +2147,15 @@
         <v>6</v>
       </c>
       <c r="M40" s="10">
-        <f>V8/U8</f>
+        <f t="shared" si="6"/>
         <v>8.4370957256483923</v>
       </c>
       <c r="N40" s="10">
-        <f>P25/U8</f>
+        <f t="shared" si="7"/>
         <v>8.184729101723681</v>
       </c>
       <c r="O40" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3.0833839555125118</v>
       </c>
     </row>
@@ -2180,15 +2180,15 @@
         <v>7</v>
       </c>
       <c r="M41" s="10">
-        <f>V9/U9</f>
+        <f t="shared" si="6"/>
         <v>21.381212399429028</v>
       </c>
       <c r="N41" s="10">
-        <f>P26/U9</f>
+        <f t="shared" si="7"/>
         <v>20.91982412767079</v>
       </c>
       <c r="O41" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2.2055074122155607</v>
       </c>
     </row>
@@ -2213,15 +2213,15 @@
         <v>8</v>
       </c>
       <c r="M42" s="10">
-        <f>V10/U10</f>
+        <f t="shared" si="6"/>
         <v>20.634675989888891</v>
       </c>
       <c r="N42" s="10">
-        <f>P27/U10</f>
+        <f t="shared" si="7"/>
         <v>20.219557791613568</v>
       </c>
       <c r="O42" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2.0530528043867546</v>
       </c>
     </row>
@@ -2247,15 +2247,15 @@
         <v>9</v>
       </c>
       <c r="M43" s="10">
-        <f>V11/U11</f>
+        <f t="shared" si="6"/>
         <v>3.6895417788735978</v>
       </c>
       <c r="N43" s="10">
-        <f>P28/U11</f>
+        <f t="shared" si="7"/>
         <v>3.5475530765375241</v>
       </c>
       <c r="O43" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>4.0024405350027141</v>
       </c>
     </row>
@@ -2281,15 +2281,15 @@
         <v>10</v>
       </c>
       <c r="M44" s="10">
-        <f>V12/U12</f>
+        <f t="shared" si="6"/>
         <v>3.1159049913413193</v>
       </c>
       <c r="N44" s="10">
-        <f>P29/U12</f>
+        <f t="shared" si="7"/>
         <v>2.9967284597821839</v>
       </c>
       <c r="O44" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3.9768879015417244</v>
       </c>
     </row>
@@ -2315,15 +2315,15 @@
         <v>11</v>
       </c>
       <c r="M45" s="10">
-        <f>V13/U13</f>
+        <f t="shared" si="6"/>
         <v>1.7698524612737996</v>
       </c>
       <c r="N45" s="10">
-        <f>P30/U13</f>
+        <f t="shared" si="7"/>
         <v>1.7229102369794462</v>
       </c>
       <c r="O45" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2.724589086930671</v>
       </c>
     </row>

</xml_diff>